<commit_message>
questionstats + devops grid action changes
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
+++ b/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14430" windowHeight="7620" activeTab="1"/>
+    <workbookView windowWidth="8775" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="assessment_grid_actions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="188">
   <si>
     <t>TestCases</t>
   </si>
@@ -174,153 +174,153 @@
     <t>Dry run evaluation through AI</t>
   </si>
   <si>
+    <t>Assessment applicants (Attended not evaluated)</t>
+  </si>
+  <si>
+    <t>View Test Status</t>
+  </si>
+  <si>
+    <t>View Candidate Transcript Old</t>
+  </si>
+  <si>
+    <t>Download Resume(s)</t>
+  </si>
+  <si>
+    <t>View Login Info</t>
+  </si>
+  <si>
+    <t>Evaluate Candidate(s)</t>
+  </si>
+  <si>
+    <t>PDF Transcript Report Old</t>
+  </si>
+  <si>
+    <t>Evaluate Manually</t>
+  </si>
+  <si>
+    <t>Online Proctoring Review</t>
+  </si>
+  <si>
+    <t>Send SMS</t>
+  </si>
+  <si>
+    <t>Send Whatsapp Message</t>
+  </si>
+  <si>
+    <t>Download Assessment Docket(s)</t>
+  </si>
+  <si>
+    <t>Remove Vendor Test Results</t>
+  </si>
+  <si>
+    <t>Invite to Retest</t>
+  </si>
+  <si>
+    <t>Force Evaluate Proctoring</t>
+  </si>
+  <si>
+    <t>Live Proctoring PDF Report</t>
+  </si>
+  <si>
+    <t>View Test User Comminications</t>
+  </si>
+  <si>
+    <t>Force Un-Tag, Tag, Send Credentials</t>
+  </si>
+  <si>
+    <t>Terminate FSA Containers</t>
+  </si>
+  <si>
+    <t>Force Re-initiate Automation</t>
+  </si>
+  <si>
+    <t>Registration Communication Status</t>
+  </si>
+  <si>
+    <t>View Registration Link</t>
+  </si>
+  <si>
+    <t>Assessment applicants (Not Attended)</t>
+  </si>
+  <si>
+    <t>Un-Tag Candidate(s)</t>
+  </si>
+  <si>
+    <t>Send Credentials</t>
+  </si>
+  <si>
+    <t>Candidate Credentials</t>
+  </si>
+  <si>
+    <t>Disable Test User</t>
+  </si>
+  <si>
+    <t>View Test Link</t>
+  </si>
+  <si>
+    <t>Send Reminder</t>
+  </si>
+  <si>
+    <t>Assessment applicants (Attending)</t>
+  </si>
+  <si>
+    <t>Configure Grace Time</t>
+  </si>
+  <si>
+    <t>Force Reactivate Test User</t>
+  </si>
+  <si>
+    <t>Force Submit</t>
+  </si>
+  <si>
+    <t>Assessment applicants (Password Disabled)</t>
+  </si>
+  <si>
+    <t>Reactivate Login</t>
+  </si>
+  <si>
     <t>Assessment applicants (Attented evaluated)</t>
   </si>
   <si>
-    <t>View Test Status</t>
-  </si>
-  <si>
-    <t>View Candidate Transcript Old</t>
-  </si>
-  <si>
     <t>View Candidate Transcript</t>
   </si>
   <si>
-    <t>Download Resume(s)</t>
-  </si>
-  <si>
-    <t>View Login Info</t>
-  </si>
-  <si>
     <t>Re-Evaluate Candidate(s)</t>
   </si>
   <si>
-    <t>PDF Transcript Report Old</t>
-  </si>
-  <si>
-    <t>Evaluate Manually</t>
-  </si>
-  <si>
-    <t>Online Proctoring Review</t>
-  </si>
-  <si>
-    <t>Send SMS</t>
-  </si>
-  <si>
-    <t>Send Whatsapp Message</t>
-  </si>
-  <si>
     <t>PDF Transcript Report</t>
   </si>
   <si>
-    <t>Download Assessment Docket(s)</t>
-  </si>
-  <si>
-    <t>Remove Vendor Test Results</t>
-  </si>
-  <si>
-    <t>Invite to Retest</t>
-  </si>
-  <si>
-    <t>Force Evaluate Proctoring</t>
-  </si>
-  <si>
     <t>View Sharable Transcript Link</t>
   </si>
   <si>
     <t>Share Transcript Link</t>
   </si>
   <si>
-    <t>Live Proctoring PDF Report</t>
-  </si>
-  <si>
     <t>Send Transcript To Candidate</t>
   </si>
   <si>
-    <t>View Test User Comminications</t>
-  </si>
-  <si>
-    <t>Force Un-Tag, Tag, Send Credentials</t>
-  </si>
-  <si>
-    <t>Terminate FSA Containers</t>
-  </si>
-  <si>
     <t>Download Web Transcript PDF</t>
   </si>
   <si>
-    <t>Force Re-initiate Automation</t>
-  </si>
-  <si>
-    <t>Registration Communication Status</t>
-  </si>
-  <si>
-    <t>View Registration Link</t>
-  </si>
-  <si>
-    <t>Assessment applicants (Attended not evaluated)</t>
-  </si>
-  <si>
-    <t>Evaluate Candidate(s)</t>
-  </si>
-  <si>
-    <t>Assessment applicants (Password Disabled)</t>
-  </si>
-  <si>
-    <t>Reactivate Login</t>
-  </si>
-  <si>
-    <t>Candidate Credentials</t>
-  </si>
-  <si>
-    <t>Configure Grace Time</t>
-  </si>
-  <si>
-    <t>View Test Link</t>
-  </si>
-  <si>
-    <t>Assessment applicants (Attending)</t>
-  </si>
-  <si>
-    <t>Force Reactivate Test User</t>
-  </si>
-  <si>
-    <t>Force Submit</t>
-  </si>
-  <si>
-    <t>Assessment applicants (Not Attended)</t>
-  </si>
-  <si>
-    <t>Un-Tag Candidate(s)</t>
-  </si>
-  <si>
-    <t>Send Credentials</t>
-  </si>
-  <si>
-    <t>Disable Test User</t>
-  </si>
-  <si>
-    <t>Send Reminder</t>
-  </si>
-  <si>
     <t>Vendor assessment grid actions</t>
   </si>
   <si>
     <t>Score Report</t>
   </si>
   <si>
+    <t>Vendor applicants (Not Attended)</t>
+  </si>
+  <si>
+    <t>Force Un-Tag (Versant)</t>
+  </si>
+  <si>
     <t>Vendor applicants (Attended)</t>
   </si>
   <si>
     <t>Candidate PDF Report</t>
   </si>
   <si>
-    <t>Vendor applicants (Not Attended)</t>
-  </si>
-  <si>
-    <t>Force Un-Tag (Versant)</t>
-  </si>
-  <si>
     <t>Event grid actions</t>
   </si>
   <si>
@@ -336,24 +336,24 @@
     <t>Manage Candidates (Partner Application)</t>
   </si>
   <si>
+    <t>Event assessment applicants (Attended not evaluated)</t>
+  </si>
+  <si>
+    <t>View Recorded Video</t>
+  </si>
+  <si>
+    <t>Event assessment applicants (Not Attended)</t>
+  </si>
+  <si>
+    <t>Event assessment applicants (Attending)</t>
+  </si>
+  <si>
+    <t>Event assessment applicants (Password Disabled)</t>
+  </si>
+  <si>
     <t>Event assessment applicants (Attented evaluated)</t>
   </si>
   <si>
-    <t>View Recorded Video</t>
-  </si>
-  <si>
-    <t>Event assessment applicants (Attended not evaluated)</t>
-  </si>
-  <si>
-    <t>Event assessment applicants (Password Disabled)</t>
-  </si>
-  <si>
-    <t>Event assessment applicants (Attending)</t>
-  </si>
-  <si>
-    <t>Event assessment applicants (Not Attended)</t>
-  </si>
-  <si>
     <t>Assessment candidates (Attented evaluated)</t>
   </si>
   <si>
@@ -363,16 +363,40 @@
     <t>View Automation Details</t>
   </si>
   <si>
+    <t>Assessment candidates (Password Disabled)</t>
+  </si>
+  <si>
+    <t>Assessment candidates (Attending)</t>
+  </si>
+  <si>
+    <t>Assessment candidates (Not Attended)</t>
+  </si>
+  <si>
     <t>Assessment candidates (Attended not evaluated)</t>
   </si>
   <si>
-    <t>Assessment candidates (Password Disabled)</t>
-  </si>
-  <si>
-    <t>Assessment candidates (Attending)</t>
-  </si>
-  <si>
-    <t>Assessment candidates (Not Attended)</t>
+    <t>Devops Assessment grid actions</t>
+  </si>
+  <si>
+    <t>Devops Assessment applicants (Attented not evaluated)</t>
+  </si>
+  <si>
+    <t>View Terminal</t>
+  </si>
+  <si>
+    <t>Reinitialize Container</t>
+  </si>
+  <si>
+    <t>Devops Assessment applicants (Attending)</t>
+  </si>
+  <si>
+    <t>Warm &amp; Pre-launch Terminal</t>
+  </si>
+  <si>
+    <t>Devops Assessment applicants (Not Attended)</t>
+  </si>
+  <si>
+    <t>Devops Assessment applicants (Attended)</t>
   </si>
   <si>
     <t>ID</t>
@@ -1529,10 +1553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AU21"/>
+  <dimension ref="A1:AU26"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" zoomScale="15" zoomScaleNormal="15" workbookViewId="0">
+      <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1701,7 +1725,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" customFormat="1" spans="1:31">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1712,10 +1736,10 @@
         <v>18603</v>
       </c>
       <c r="D3">
-        <v>3774865</v>
+        <v>3778101</v>
       </c>
       <c r="E3">
-        <v>1564087</v>
+        <v>1565333</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -1751,10 +1775,10 @@
         <v>58</v>
       </c>
       <c r="Q3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s">
         <v>59</v>
-      </c>
-      <c r="R3" t="s">
-        <v>33</v>
       </c>
       <c r="S3" t="s">
         <v>60</v>
@@ -1763,13 +1787,13 @@
         <v>61</v>
       </c>
       <c r="U3" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" t="s">
         <v>62</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>63</v>
-      </c>
-      <c r="W3" t="s">
-        <v>39</v>
       </c>
       <c r="X3" t="s">
         <v>64</v>
@@ -1781,42 +1805,24 @@
         <v>66</v>
       </c>
       <c r="AA3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB3" t="s">
         <v>67</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>68</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>69</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" spans="1:25">
+      <c r="A4" t="s">
         <v>70</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>75</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" customFormat="1" spans="1:31">
-      <c r="A4" t="s">
-        <v>76</v>
       </c>
       <c r="B4">
         <v>21193</v>
@@ -1825,10 +1831,10 @@
         <v>18603</v>
       </c>
       <c r="D4">
-        <v>3778101</v>
+        <v>3774871</v>
       </c>
       <c r="E4">
-        <v>1565333</v>
+        <v>1564095</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -1837,81 +1843,63 @@
         <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="R4" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="S4" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U4" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="V4" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="W4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
         <v>69</v>
       </c>
       <c r="Y4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AE4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:28">
+    <row r="5" customFormat="1" spans="1:30">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>21193</v>
@@ -1920,10 +1908,10 @@
         <v>18603</v>
       </c>
       <c r="D5">
-        <v>3774867</v>
+        <v>3774869</v>
       </c>
       <c r="E5">
-        <v>1564089</v>
+        <v>1564093</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -1932,34 +1920,34 @@
         <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" t="s">
         <v>57</v>
-      </c>
-      <c r="L5" t="s">
-        <v>80</v>
       </c>
       <c r="M5" t="s">
         <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="O5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="R5" t="s">
         <v>12</v>
@@ -1968,36 +1956,42 @@
         <v>39</v>
       </c>
       <c r="T5" t="s">
+        <v>62</v>
+      </c>
+      <c r="U5" t="s">
+        <v>80</v>
+      </c>
+      <c r="V5" t="s">
+        <v>63</v>
+      </c>
+      <c r="W5" t="s">
         <v>64</v>
       </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA5" t="s">
         <v>67</v>
       </c>
-      <c r="V5" t="s">
+      <c r="AB5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC5" t="s">
         <v>69</v>
       </c>
-      <c r="W5" t="s">
-        <v>70</v>
-      </c>
-      <c r="X5" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>75</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="AD5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" customFormat="1" spans="1:30">
+    <row r="6" customFormat="1" spans="1:28">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>21193</v>
@@ -2006,10 +2000,10 @@
         <v>18603</v>
       </c>
       <c r="D6">
-        <v>3774869</v>
+        <v>3774867</v>
       </c>
       <c r="E6">
-        <v>1564093</v>
+        <v>1564089</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
@@ -2018,34 +2012,34 @@
         <v>49</v>
       </c>
       <c r="H6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L6" t="s">
+        <v>73</v>
+      </c>
+      <c r="M6" t="s">
         <v>57</v>
       </c>
-      <c r="K6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>58</v>
       </c>
-      <c r="M6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N6" t="s">
-        <v>81</v>
-      </c>
       <c r="O6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="P6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="R6" t="s">
         <v>12</v>
@@ -2054,42 +2048,36 @@
         <v>39</v>
       </c>
       <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" t="s">
         <v>64</v>
       </c>
-      <c r="U6" t="s">
-        <v>85</v>
-      </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
+        <v>65</v>
+      </c>
+      <c r="X6" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" t="s">
         <v>67</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Z6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" t="s">
         <v>69</v>
       </c>
-      <c r="X6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>73</v>
-      </c>
       <c r="AB6" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>75</v>
-      </c>
-      <c r="AD6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" customFormat="1" spans="1:25">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>21193</v>
@@ -2098,10 +2086,10 @@
         <v>18603</v>
       </c>
       <c r="D7">
-        <v>3774871</v>
+        <v>3774865</v>
       </c>
       <c r="E7">
-        <v>1564095</v>
+        <v>1564087</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
@@ -2110,57 +2098,93 @@
         <v>49</v>
       </c>
       <c r="H7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
         <v>52</v>
       </c>
-      <c r="I7" t="s">
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" t="s">
+        <v>86</v>
+      </c>
+      <c r="T7" t="s">
+        <v>59</v>
+      </c>
+      <c r="U7" t="s">
+        <v>60</v>
+      </c>
+      <c r="V7" t="s">
+        <v>61</v>
+      </c>
+      <c r="W7" t="s">
+        <v>39</v>
+      </c>
+      <c r="X7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y7" t="s">
         <v>87</v>
       </c>
-      <c r="J7" t="s">
+      <c r="Z7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="AA7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB7" t="s">
         <v>89</v>
       </c>
-      <c r="O7" t="s">
-        <v>62</v>
-      </c>
-      <c r="P7" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="AC7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG7" t="s">
         <v>90</v>
       </c>
-      <c r="S7" t="s">
-        <v>30</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="AH7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ7" t="s">
         <v>69</v>
       </c>
-      <c r="U7" t="s">
-        <v>70</v>
-      </c>
-      <c r="V7" t="s">
-        <v>46</v>
-      </c>
-      <c r="W7" t="s">
-        <v>74</v>
-      </c>
-      <c r="X7" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y7" t="s">
+      <c r="AK7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2307,7 +2331,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:32">
+    <row r="9" customFormat="1" spans="1:26">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2318,10 +2342,10 @@
         <v>18829</v>
       </c>
       <c r="D9">
-        <v>3778097</v>
+        <v>3778099</v>
       </c>
       <c r="E9">
-        <v>1565335</v>
+        <v>1565337</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -2330,52 +2354,52 @@
         <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="Q9" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="S9" t="s">
+        <v>30</v>
+      </c>
+      <c r="T9" t="s">
+        <v>64</v>
+      </c>
+      <c r="U9" t="s">
         <v>94</v>
       </c>
-      <c r="T9" t="s">
-        <v>63</v>
-      </c>
-      <c r="U9" t="s">
-        <v>39</v>
-      </c>
       <c r="V9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W9" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="X9" t="s">
         <v>68</v>
@@ -2384,28 +2408,10 @@
         <v>69</v>
       </c>
       <c r="Z9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:26">
+    <row r="10" customFormat="1" spans="1:32">
       <c r="A10" t="s">
         <v>95</v>
       </c>
@@ -2416,10 +2422,10 @@
         <v>18829</v>
       </c>
       <c r="D10">
-        <v>3778099</v>
+        <v>3778097</v>
       </c>
       <c r="E10">
-        <v>1565337</v>
+        <v>1565335</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
@@ -2428,60 +2434,78 @@
         <v>49</v>
       </c>
       <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" t="s">
         <v>52</v>
       </c>
-      <c r="I10" t="s">
-        <v>87</v>
-      </c>
-      <c r="J10" t="s">
-        <v>88</v>
-      </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M10" t="s">
+        <v>56</v>
+      </c>
+      <c r="N10" t="s">
+        <v>57</v>
+      </c>
+      <c r="O10" t="s">
         <v>58</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q10" t="s">
         <v>59</v>
       </c>
-      <c r="N10" t="s">
+      <c r="R10" t="s">
+        <v>60</v>
+      </c>
+      <c r="S10" t="s">
+        <v>96</v>
+      </c>
+      <c r="T10" t="s">
+        <v>61</v>
+      </c>
+      <c r="U10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" t="s">
+        <v>62</v>
+      </c>
+      <c r="W10" t="s">
+        <v>63</v>
+      </c>
+      <c r="X10" t="s">
         <v>89</v>
       </c>
-      <c r="O10" t="s">
-        <v>62</v>
-      </c>
-      <c r="P10" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>12</v>
-      </c>
-      <c r="R10" t="s">
-        <v>90</v>
-      </c>
-      <c r="S10" t="s">
-        <v>30</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="Y10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE10" t="s">
         <v>69</v>
       </c>
-      <c r="U10" t="s">
-        <v>96</v>
-      </c>
-      <c r="V10" t="s">
-        <v>70</v>
-      </c>
-      <c r="W10" t="s">
-        <v>46</v>
-      </c>
-      <c r="X10" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z10" t="s">
+      <c r="AF10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2580,7 +2604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>102</v>
       </c>
@@ -2621,52 +2645,40 @@
         <v>55</v>
       </c>
       <c r="N12" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="O12" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="P12" t="s">
         <v>58</v>
       </c>
       <c r="Q12" t="s">
+        <v>33</v>
+      </c>
+      <c r="R12" t="s">
         <v>59</v>
       </c>
-      <c r="R12" t="s">
-        <v>33</v>
-      </c>
       <c r="S12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" t="s">
         <v>60</v>
       </c>
-      <c r="T12" t="s">
-        <v>61</v>
-      </c>
       <c r="U12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="V12" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="W12" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="X12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y12" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA12" t="s">
         <v>47</v>
       </c>
-      <c r="AB12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -2689,58 +2701,49 @@
         <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="L13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="M13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="O13" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="Q13" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="R13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S13" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="T13" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="U13" t="s">
-        <v>71</v>
-      </c>
-      <c r="V13" t="s">
-        <v>73</v>
-      </c>
-      <c r="W13" t="s">
-        <v>46</v>
-      </c>
-      <c r="X13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -2763,49 +2766,55 @@
         <v>49</v>
       </c>
       <c r="H14" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="I14" t="s">
         <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="K14" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
         <v>58</v>
       </c>
       <c r="N14" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="O14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="Q14" t="s">
         <v>12</v>
       </c>
       <c r="R14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S14" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="T14" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" t="s">
+        <v>67</v>
+      </c>
+      <c r="V14" t="s">
         <v>46</v>
       </c>
-      <c r="U14" t="s">
+      <c r="W14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -2828,55 +2837,49 @@
         <v>49</v>
       </c>
       <c r="H15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" t="s">
         <v>52</v>
       </c>
-      <c r="I15" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>103</v>
       </c>
-      <c r="K15" t="s">
-        <v>80</v>
-      </c>
       <c r="L15" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" t="s">
         <v>58</v>
       </c>
-      <c r="M15" t="s">
-        <v>59</v>
-      </c>
-      <c r="N15" t="s">
-        <v>81</v>
-      </c>
       <c r="O15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="P15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="Q15" t="s">
         <v>12</v>
       </c>
       <c r="R15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S15" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="T15" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="U15" t="s">
-        <v>73</v>
-      </c>
-      <c r="V15" t="s">
-        <v>46</v>
-      </c>
-      <c r="W15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:28">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2899,46 +2902,67 @@
         <v>49</v>
       </c>
       <c r="H16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
         <v>52</v>
       </c>
-      <c r="I16" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" t="s">
-        <v>88</v>
-      </c>
-      <c r="K16" t="s">
-        <v>80</v>
-      </c>
       <c r="L16" t="s">
+        <v>85</v>
+      </c>
+      <c r="M16" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" t="s">
+        <v>55</v>
+      </c>
+      <c r="O16" t="s">
+        <v>103</v>
+      </c>
+      <c r="P16" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q16" t="s">
         <v>58</v>
       </c>
-      <c r="M16" t="s">
+      <c r="R16" t="s">
+        <v>33</v>
+      </c>
+      <c r="S16" t="s">
+        <v>86</v>
+      </c>
+      <c r="T16" t="s">
         <v>59</v>
       </c>
-      <c r="N16" t="s">
+      <c r="U16" t="s">
+        <v>61</v>
+      </c>
+      <c r="V16" t="s">
+        <v>60</v>
+      </c>
+      <c r="W16" t="s">
         <v>89</v>
       </c>
-      <c r="O16" t="s">
-        <v>82</v>
-      </c>
-      <c r="P16" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="X16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB16" t="s">
         <v>90</v>
-      </c>
-      <c r="R16" t="s">
-        <v>62</v>
-      </c>
-      <c r="S16" t="s">
-        <v>30</v>
-      </c>
-      <c r="T16" t="s">
-        <v>46</v>
-      </c>
-      <c r="U16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -2961,34 +2985,34 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
         <v>109</v>
       </c>
       <c r="I17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
         <v>39</v>
       </c>
       <c r="K17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L17" t="s">
         <v>110</v>
       </c>
       <c r="M17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="O17" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="P17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="Q17" t="s">
         <v>47</v>
@@ -2997,7 +3021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -3008,55 +3032,49 @@
         <v>18603</v>
       </c>
       <c r="D18">
-        <v>3778101</v>
+        <v>3774867</v>
       </c>
       <c r="E18">
-        <v>1565333</v>
+        <v>1564089</v>
       </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
         <v>109</v>
       </c>
       <c r="J18" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="K18" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
+        <v>110</v>
+      </c>
+      <c r="M18" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" t="s">
         <v>64</v>
       </c>
-      <c r="M18" t="s">
-        <v>110</v>
-      </c>
-      <c r="N18" t="s">
-        <v>59</v>
-      </c>
       <c r="O18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P18" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="Q18" t="s">
-        <v>73</v>
-      </c>
-      <c r="R18" t="s">
-        <v>47</v>
-      </c>
-      <c r="S18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:19">
       <c r="A19" t="s">
         <v>112</v>
       </c>
@@ -3067,19 +3085,19 @@
         <v>18603</v>
       </c>
       <c r="D19">
-        <v>3774867</v>
+        <v>3774869</v>
       </c>
       <c r="E19">
-        <v>1564089</v>
+        <v>1564093</v>
       </c>
       <c r="F19" t="s">
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
         <v>109</v>
@@ -3088,28 +3106,34 @@
         <v>39</v>
       </c>
       <c r="K19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
         <v>110</v>
       </c>
       <c r="M19" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="N19" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="O19" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="P19" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>67</v>
+      </c>
+      <c r="R19" t="s">
         <v>47</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="S19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>113</v>
       </c>
@@ -3120,55 +3144,46 @@
         <v>18603</v>
       </c>
       <c r="D20">
-        <v>3774869</v>
+        <v>3774871</v>
       </c>
       <c r="E20">
-        <v>1564093</v>
+        <v>1564095</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
+        <v>110</v>
+      </c>
+      <c r="L20" t="s">
+        <v>58</v>
+      </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" t="s">
         <v>64</v>
       </c>
-      <c r="L20" t="s">
-        <v>110</v>
-      </c>
-      <c r="M20" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20" t="s">
-        <v>59</v>
-      </c>
       <c r="O20" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="P20" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>73</v>
-      </c>
-      <c r="R20" t="s">
-        <v>47</v>
-      </c>
-      <c r="S20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:19">
       <c r="A21" t="s">
         <v>114</v>
       </c>
@@ -3179,43 +3194,572 @@
         <v>18603</v>
       </c>
       <c r="D21">
-        <v>3774871</v>
+        <v>3778101</v>
       </c>
       <c r="E21">
-        <v>1564095</v>
+        <v>1565333</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" t="s">
         <v>109</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
+        <v>61</v>
+      </c>
+      <c r="K21" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" t="s">
+        <v>110</v>
+      </c>
+      <c r="N21" t="s">
+        <v>58</v>
+      </c>
+      <c r="O21" t="s">
+        <v>64</v>
+      </c>
+      <c r="P21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>67</v>
+      </c>
+      <c r="R21" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46">
+      <c r="A22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22">
+        <v>21193</v>
+      </c>
+      <c r="C22">
+        <v>18603</v>
+      </c>
+      <c r="D22">
+        <v>3774865</v>
+      </c>
+      <c r="E22">
+        <v>1564087</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
         <v>12</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" t="s">
+        <v>14</v>
+      </c>
+      <c r="N22" t="s">
+        <v>15</v>
+      </c>
+      <c r="O22" t="s">
+        <v>16</v>
+      </c>
+      <c r="P22" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>18</v>
+      </c>
+      <c r="R22" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22" t="s">
+        <v>20</v>
+      </c>
+      <c r="T22" t="s">
+        <v>21</v>
+      </c>
+      <c r="U22" t="s">
+        <v>22</v>
+      </c>
+      <c r="V22" t="s">
+        <v>23</v>
+      </c>
+      <c r="W22" t="s">
+        <v>24</v>
+      </c>
+      <c r="X22" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ22" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK22" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL22" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO22" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP22" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS22" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" spans="1:30">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23">
+        <v>21193</v>
+      </c>
+      <c r="C23">
+        <v>18603</v>
+      </c>
+      <c r="D23">
+        <v>3778101</v>
+      </c>
+      <c r="E23">
+        <v>1565333</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" t="s">
+        <v>52</v>
+      </c>
+      <c r="K23" t="s">
+        <v>53</v>
+      </c>
+      <c r="L23" t="s">
+        <v>54</v>
+      </c>
+      <c r="M23" t="s">
+        <v>56</v>
+      </c>
+      <c r="N23" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" t="s">
+        <v>58</v>
+      </c>
+      <c r="P23" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>59</v>
+      </c>
+      <c r="R23" t="s">
+        <v>60</v>
+      </c>
+      <c r="S23" t="s">
+        <v>61</v>
+      </c>
+      <c r="T23" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" t="s">
+        <v>64</v>
+      </c>
+      <c r="V23" t="s">
+        <v>65</v>
+      </c>
+      <c r="W23" t="s">
+        <v>66</v>
+      </c>
+      <c r="X23" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" spans="1:31">
+      <c r="A24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24">
+        <v>21193</v>
+      </c>
+      <c r="C24">
+        <v>18603</v>
+      </c>
+      <c r="D24">
+        <v>3774869</v>
+      </c>
+      <c r="E24">
+        <v>1564093</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K24" t="s">
+        <v>73</v>
+      </c>
+      <c r="L24" t="s">
+        <v>57</v>
+      </c>
+      <c r="M24" t="s">
+        <v>58</v>
+      </c>
+      <c r="N24" t="s">
+        <v>78</v>
+      </c>
+      <c r="O24" t="s">
+        <v>79</v>
+      </c>
+      <c r="P24" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>75</v>
+      </c>
+      <c r="R24" t="s">
+        <v>12</v>
+      </c>
+      <c r="S24" t="s">
+        <v>80</v>
+      </c>
+      <c r="T24" t="s">
+        <v>63</v>
+      </c>
+      <c r="U24" t="s">
+        <v>64</v>
+      </c>
+      <c r="V24" t="s">
+        <v>65</v>
+      </c>
+      <c r="W24" t="s">
+        <v>66</v>
+      </c>
+      <c r="X24" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>118</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" spans="1:27">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25">
+        <v>21193</v>
+      </c>
+      <c r="C25">
+        <v>18603</v>
+      </c>
+      <c r="D25">
+        <v>3774871</v>
+      </c>
+      <c r="E25">
+        <v>1564095</v>
+      </c>
+      <c r="F25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L25" t="s">
+        <v>57</v>
+      </c>
+      <c r="M25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N25" t="s">
+        <v>74</v>
+      </c>
+      <c r="O25" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" t="s">
+        <v>76</v>
+      </c>
+      <c r="S25" t="s">
+        <v>30</v>
+      </c>
+      <c r="T25" t="s">
+        <v>64</v>
+      </c>
+      <c r="U25" t="s">
+        <v>65</v>
+      </c>
+      <c r="V25" t="s">
+        <v>46</v>
+      </c>
+      <c r="W25" t="s">
+        <v>68</v>
+      </c>
+      <c r="X25" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" spans="1:36">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26">
+        <v>21193</v>
+      </c>
+      <c r="C26">
+        <v>18603</v>
+      </c>
+      <c r="D26">
+        <v>3774865</v>
+      </c>
+      <c r="E26">
+        <v>1564087</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" t="s">
+        <v>84</v>
+      </c>
+      <c r="J26" t="s">
+        <v>51</v>
+      </c>
+      <c r="K26" t="s">
+        <v>52</v>
+      </c>
+      <c r="L26" t="s">
+        <v>85</v>
+      </c>
+      <c r="M26" t="s">
+        <v>54</v>
+      </c>
+      <c r="N26" t="s">
+        <v>56</v>
+      </c>
+      <c r="O26" t="s">
+        <v>57</v>
+      </c>
+      <c r="P26" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>33</v>
+      </c>
+      <c r="R26" t="s">
+        <v>86</v>
+      </c>
+      <c r="S26" t="s">
+        <v>59</v>
+      </c>
+      <c r="T26" t="s">
+        <v>60</v>
+      </c>
+      <c r="U26" t="s">
+        <v>61</v>
+      </c>
+      <c r="V26" t="s">
+        <v>87</v>
+      </c>
+      <c r="W26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X26" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD26" t="s">
         <v>90</v>
       </c>
-      <c r="K21" t="s">
-        <v>110</v>
-      </c>
-      <c r="L21" t="s">
-        <v>59</v>
-      </c>
-      <c r="M21" t="s">
-        <v>30</v>
-      </c>
-      <c r="N21" t="s">
+      <c r="AE26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG26" t="s">
         <v>69</v>
       </c>
-      <c r="O21" t="s">
+      <c r="AH26" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ26" t="s">
         <v>47</v>
-      </c>
-      <c r="P21" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -3229,8 +3773,8 @@
   <sheetPr/>
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3244,967 +3788,967 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B2">
         <v>3795</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="B3">
         <v>3743</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B4">
         <v>14105</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="H4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="I4" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="J4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="L4" t="s">
         <v>40</v>
       </c>
       <c r="M4" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="N4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="O4" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>14103</v>
       </c>
       <c r="C5" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
         <v>134</v>
       </c>
-      <c r="E5" t="s">
-        <v>126</v>
-      </c>
       <c r="F5" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="I5" t="s">
         <v>40</v>
       </c>
       <c r="J5" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="K5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="L5" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B6">
         <v>147813</v>
       </c>
       <c r="C6" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D6" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B7">
         <v>147809</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G7" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H7" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B8">
         <v>147807</v>
       </c>
       <c r="C8" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F8" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H8" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I8" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B9">
         <v>147805</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D9" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G9" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I9" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B10">
         <v>147801</v>
       </c>
       <c r="C10" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" t="s">
         <v>147</v>
       </c>
-      <c r="G10" t="s">
-        <v>144</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>148</v>
       </c>
-      <c r="I10" t="s">
-        <v>139</v>
-      </c>
-      <c r="J10" t="s">
-        <v>140</v>
-      </c>
       <c r="K10" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B11">
         <v>147799</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F11" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="G11" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H11" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="J11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="B12">
         <v>147797</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D12" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="H12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I12" t="s">
         <v>147</v>
       </c>
-      <c r="G12" t="s">
+      <c r="J12" t="s">
         <v>148</v>
       </c>
-      <c r="H12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J12" t="s">
-        <v>140</v>
-      </c>
       <c r="K12" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="B13">
         <v>147795</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G13" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H13" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I13" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B14">
         <v>147793</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F14" t="s">
+        <v>155</v>
+      </c>
+      <c r="G14" t="s">
         <v>147</v>
       </c>
-      <c r="G14" t="s">
-        <v>139</v>
-      </c>
       <c r="H14" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I14" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B15">
         <v>147789</v>
       </c>
       <c r="C15" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
+        <v>155</v>
+      </c>
+      <c r="F15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G15" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" t="s">
         <v>147</v>
       </c>
-      <c r="F15" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>148</v>
       </c>
-      <c r="H15" t="s">
-        <v>139</v>
-      </c>
-      <c r="I15" t="s">
-        <v>140</v>
-      </c>
       <c r="J15" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B16">
         <v>147787</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" t="s">
+        <v>156</v>
+      </c>
+      <c r="I16" t="s">
         <v>147</v>
       </c>
-      <c r="G16" t="s">
-        <v>144</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>148</v>
       </c>
-      <c r="I16" t="s">
-        <v>139</v>
-      </c>
-      <c r="J16" t="s">
-        <v>140</v>
-      </c>
       <c r="K16" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="B17">
         <v>147785</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F17" t="s">
+        <v>155</v>
+      </c>
+      <c r="G17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" t="s">
+        <v>156</v>
+      </c>
+      <c r="I17" t="s">
         <v>147</v>
       </c>
-      <c r="G17" t="s">
-        <v>144</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>148</v>
       </c>
-      <c r="I17" t="s">
-        <v>139</v>
-      </c>
-      <c r="J17" t="s">
-        <v>140</v>
-      </c>
       <c r="K17" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B18">
         <v>147783</v>
       </c>
       <c r="C18" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F18" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I18" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="B19">
         <v>147781</v>
       </c>
       <c r="C19" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G19" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="H19" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="I19" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B20">
         <v>147779</v>
       </c>
       <c r="C20" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F20" t="s">
+        <v>155</v>
+      </c>
+      <c r="G20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H20" t="s">
         <v>147</v>
       </c>
-      <c r="G20" t="s">
-        <v>144</v>
-      </c>
-      <c r="H20" t="s">
-        <v>139</v>
-      </c>
       <c r="I20" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B21">
         <v>147771</v>
       </c>
       <c r="C21" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" t="s">
         <v>147</v>
       </c>
-      <c r="G21" t="s">
-        <v>144</v>
-      </c>
-      <c r="H21" t="s">
-        <v>163</v>
-      </c>
-      <c r="I21" t="s">
-        <v>139</v>
-      </c>
       <c r="J21" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="K21" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B22">
         <v>147763</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D22" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E22" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" t="s">
+        <v>156</v>
+      </c>
+      <c r="I22" t="s">
         <v>147</v>
       </c>
-      <c r="G22" t="s">
-        <v>144</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>148</v>
       </c>
-      <c r="I22" t="s">
-        <v>139</v>
-      </c>
-      <c r="J22" t="s">
-        <v>140</v>
-      </c>
       <c r="K22" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="L22" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B23">
         <v>147761</v>
       </c>
       <c r="C23" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D23" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H23" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" t="s">
         <v>148</v>
       </c>
-      <c r="I23" t="s">
-        <v>140</v>
-      </c>
       <c r="J23" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K23" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B24">
         <v>147759</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E24" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
+        <v>155</v>
+      </c>
+      <c r="G24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H24" t="s">
         <v>147</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>148</v>
       </c>
-      <c r="H24" t="s">
-        <v>139</v>
-      </c>
-      <c r="I24" t="s">
-        <v>140</v>
-      </c>
       <c r="J24" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K24" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B25">
         <v>147757</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" t="s">
         <v>147</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>148</v>
       </c>
-      <c r="H25" t="s">
-        <v>139</v>
-      </c>
-      <c r="I25" t="s">
-        <v>140</v>
-      </c>
       <c r="J25" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="K25" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B26">
         <v>148425</v>
       </c>
       <c r="C26" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" t="s">
         <v>147</v>
       </c>
-      <c r="E26" t="s">
-        <v>139</v>
-      </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G26" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B27">
         <v>148343</v>
       </c>
       <c r="C27" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D27" t="s">
+        <v>155</v>
+      </c>
+      <c r="E27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" t="s">
         <v>147</v>
       </c>
-      <c r="E27" t="s">
-        <v>153</v>
-      </c>
-      <c r="F27" t="s">
-        <v>139</v>
-      </c>
       <c r="G27" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="H27" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B28">
         <v>148341</v>
       </c>
       <c r="C28" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" t="s">
         <v>147</v>
       </c>
-      <c r="E28" t="s">
-        <v>139</v>
-      </c>
       <c r="F28" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G28" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B29">
         <v>148339</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" t="s">
         <v>147</v>
       </c>
-      <c r="E29" t="s">
-        <v>139</v>
-      </c>
       <c r="F29" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G29" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B30">
         <v>148337</v>
       </c>
       <c r="C30" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="B31">
         <v>148335</v>
       </c>
       <c r="C31" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B32">
         <v>148333</v>
       </c>
       <c r="C32" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D32" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" t="s">
         <v>147</v>
       </c>
-      <c r="E32" t="s">
-        <v>139</v>
-      </c>
       <c r="F32" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G32" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B33">
         <v>148327</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" t="s">
         <v>147</v>
       </c>
-      <c r="E33" t="s">
-        <v>139</v>
-      </c>
       <c r="F33" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G33" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B34">
         <v>148325</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" t="s">
         <v>147</v>
       </c>
-      <c r="E34" t="s">
-        <v>139</v>
-      </c>
       <c r="F34" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G34" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="H34" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
grid actions / sanitize / selfassessment fix
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
+++ b/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView windowWidth="16575" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="assessment_grid_actions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="225">
   <si>
     <t>TestCases</t>
   </si>
@@ -107,15 +107,9 @@
     <t>Calculate Percentile</t>
   </si>
   <si>
-    <t>Mark Attending Candidates To Password Disabled</t>
-  </si>
-  <si>
     <t>Sync Candidate Email</t>
   </si>
   <si>
-    <t>Mark Submitting Candidates To Password Disabled</t>
-  </si>
-  <si>
     <t>Proctored Video</t>
   </si>
   <si>
@@ -173,6 +167,9 @@
     <t>Sanitise Test Automation</t>
   </si>
   <si>
+    <t>Update Assessment Tags</t>
+  </si>
+  <si>
     <t>Dry run evaluation through AI</t>
   </si>
   <si>
@@ -389,6 +386,12 @@
     <t>Reinitialize Container</t>
   </si>
   <si>
+    <t>Launch Evaluation Container</t>
+  </si>
+  <si>
+    <t>View And Download Candidate DevOPS Answer</t>
+  </si>
+  <si>
     <t>Devops Assessment applicants (Attending)</t>
   </si>
   <si>
@@ -443,7 +446,7 @@
     <t>View Related Tests</t>
   </si>
   <si>
-    <t>Background Task</t>
+    <t>Migrate Question Files</t>
   </si>
   <si>
     <t>View Question Statistics JSON</t>
@@ -615,6 +618,9 @@
   </si>
   <si>
     <t>Update Backend Configuration</t>
+  </si>
+  <si>
+    <t>Upload Candidates by Resume</t>
   </si>
   <si>
     <t>Password Disabled</t>
@@ -1322,7 +1328,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1660,9 +1666,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AU26"/>
+  <dimension ref="A1:AT26"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" topLeftCell="A3" workbookViewId="0">
+    <sheetView zoomScale="103" zoomScaleNormal="103" topLeftCell="X8" workbookViewId="0">
       <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:46">
+    <row r="2" spans="1:45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1828,13 +1834,10 @@
       <c r="AS2" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="3" customFormat="1" spans="1:31">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>21193</v>
@@ -1852,84 +1855,84 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>51</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>52</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>56</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>57</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" t="s">
         <v>58</v>
       </c>
-      <c r="Q3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>59</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>60</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
         <v>61</v>
       </c>
-      <c r="U3" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>62</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>63</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>65</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB3" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AC3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE3" t="s">
         <v>46</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <v>21193</v>
@@ -1947,66 +1950,66 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
         <v>71</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>72</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" t="s">
         <v>73</v>
       </c>
-      <c r="L4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" t="s">
         <v>74</v>
-      </c>
-      <c r="O4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>75</v>
       </c>
       <c r="Q4" t="s">
         <v>12</v>
       </c>
       <c r="R4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U4" t="s">
         <v>64</v>
       </c>
-      <c r="U4" t="s">
-        <v>65</v>
-      </c>
       <c r="V4" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" t="s">
+        <v>67</v>
+      </c>
+      <c r="X4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y4" t="s">
         <v>46</v>
-      </c>
-      <c r="W4" t="s">
-        <v>68</v>
-      </c>
-      <c r="X4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:30">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>21193</v>
@@ -2024,81 +2027,81 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
-        <v>52</v>
-      </c>
       <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5" t="s">
         <v>56</v>
       </c>
-      <c r="K5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>57</v>
       </c>
-      <c r="M5" t="s">
-        <v>58</v>
-      </c>
       <c r="N5" t="s">
+        <v>77</v>
+      </c>
+      <c r="O5" t="s">
         <v>78</v>
       </c>
-      <c r="O5" t="s">
-        <v>79</v>
-      </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R5" t="s">
         <v>12</v>
       </c>
       <c r="S5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T5" t="s">
+        <v>61</v>
+      </c>
+      <c r="U5" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" t="s">
         <v>62</v>
       </c>
-      <c r="U5" t="s">
-        <v>80</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>63</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>64</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>65</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA5" t="s">
         <v>66</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD5" t="s">
         <v>46</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:28">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6">
         <v>21193</v>
@@ -2116,75 +2119,75 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
         <v>51</v>
       </c>
-      <c r="J6" t="s">
-        <v>52</v>
-      </c>
       <c r="K6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>72</v>
+      </c>
+      <c r="M6" t="s">
         <v>56</v>
       </c>
-      <c r="L6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>57</v>
       </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
       <c r="O6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R6" t="s">
         <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T6" t="s">
+        <v>61</v>
+      </c>
+      <c r="U6" t="s">
         <v>62</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>63</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>64</v>
       </c>
-      <c r="W6" t="s">
-        <v>65</v>
-      </c>
       <c r="X6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB6" t="s">
         <v>46</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7">
         <v>21193</v>
@@ -2202,102 +2205,102 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>83</v>
+      </c>
+      <c r="J7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" t="s">
         <v>84</v>
       </c>
-      <c r="J7" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>57</v>
+      </c>
+      <c r="R7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S7" t="s">
         <v>85</v>
       </c>
-      <c r="M7" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" t="s">
-        <v>56</v>
-      </c>
-      <c r="P7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="T7" t="s">
         <v>58</v>
       </c>
-      <c r="R7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
+        <v>59</v>
+      </c>
+      <c r="V7" t="s">
+        <v>60</v>
+      </c>
+      <c r="W7" t="s">
+        <v>37</v>
+      </c>
+      <c r="X7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y7" t="s">
         <v>86</v>
       </c>
-      <c r="T7" t="s">
-        <v>59</v>
-      </c>
-      <c r="U7" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" t="s">
-        <v>61</v>
-      </c>
-      <c r="W7" t="s">
-        <v>39</v>
-      </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA7" t="s">
         <v>62</v>
       </c>
-      <c r="Y7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z7" t="s">
+      <c r="AB7" t="s">
         <v>88</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>63</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AD7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG7" t="s">
         <v>89</v>
       </c>
-      <c r="AC7" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE7" t="s">
+      <c r="AH7" t="s">
         <v>66</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AI7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK7" t="s">
         <v>46</v>
       </c>
-      <c r="AG7" t="s">
+    </row>
+    <row r="8" customFormat="1" spans="1:46">
+      <c r="A8" t="s">
         <v>90</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" customFormat="1" spans="1:47">
-      <c r="A8" t="s">
-        <v>91</v>
       </c>
       <c r="B8">
         <v>21381</v>
@@ -2396,13 +2399,13 @@
         <v>34</v>
       </c>
       <c r="AH8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI8" t="s">
         <v>35</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AJ8" t="s">
         <v>36</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>92</v>
       </c>
       <c r="AK8" t="s">
         <v>37</v>
@@ -2434,13 +2437,10 @@
       <c r="AT8" t="s">
         <v>46</v>
       </c>
-      <c r="AU8" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="9" customFormat="1" spans="1:26">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9">
         <v>21381</v>
@@ -2458,69 +2458,69 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
         <v>71</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>72</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N9" t="s">
         <v>73</v>
       </c>
-      <c r="L9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" t="s">
-        <v>58</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" t="s">
         <v>74</v>
-      </c>
-      <c r="O9" t="s">
-        <v>60</v>
-      </c>
-      <c r="P9" t="s">
-        <v>75</v>
       </c>
       <c r="Q9" t="s">
         <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T9" t="s">
+        <v>63</v>
+      </c>
+      <c r="U9" t="s">
+        <v>93</v>
+      </c>
+      <c r="V9" t="s">
         <v>64</v>
       </c>
-      <c r="U9" t="s">
-        <v>94</v>
-      </c>
-      <c r="V9" t="s">
-        <v>65</v>
-      </c>
       <c r="W9" t="s">
+        <v>44</v>
+      </c>
+      <c r="X9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z9" t="s">
         <v>46</v>
-      </c>
-      <c r="X9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:32">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10">
         <v>21381</v>
@@ -2538,87 +2538,87 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" t="s">
         <v>49</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>50</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>51</v>
       </c>
-      <c r="J10" t="s">
-        <v>52</v>
-      </c>
       <c r="K10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M10" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" t="s">
         <v>56</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>57</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" t="s">
         <v>58</v>
       </c>
-      <c r="P10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>59</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
+        <v>95</v>
+      </c>
+      <c r="T10" t="s">
         <v>60</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" t="s">
+        <v>61</v>
+      </c>
+      <c r="W10" t="s">
+        <v>62</v>
+      </c>
+      <c r="X10" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="A11" t="s">
         <v>96</v>
-      </c>
-      <c r="T10" t="s">
-        <v>61</v>
-      </c>
-      <c r="U10" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" t="s">
-        <v>62</v>
-      </c>
-      <c r="W10" t="s">
-        <v>63</v>
-      </c>
-      <c r="X10" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
-      <c r="A11" t="s">
-        <v>97</v>
       </c>
       <c r="B11">
         <v>21193</v>
@@ -2681,39 +2681,42 @@
         <v>24</v>
       </c>
       <c r="V11" t="s">
+        <v>25</v>
+      </c>
+      <c r="W11" t="s">
         <v>26</v>
       </c>
-      <c r="W11" t="s">
+      <c r="X11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD11" t="s">
         <v>28</v>
       </c>
-      <c r="X11" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>100</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>101</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>30</v>
-      </c>
       <c r="AE11" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12">
         <v>21193</v>
@@ -2731,63 +2734,63 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
         <v>49</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>50</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>51</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>52</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>53</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>54</v>
       </c>
-      <c r="M12" t="s">
-        <v>55</v>
-      </c>
       <c r="N12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O12" t="s">
+        <v>56</v>
+      </c>
+      <c r="P12" t="s">
         <v>57</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" t="s">
         <v>58</v>
       </c>
-      <c r="Q12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" t="s">
         <v>59</v>
       </c>
-      <c r="S12" t="s">
-        <v>61</v>
-      </c>
-      <c r="T12" t="s">
-        <v>60</v>
-      </c>
       <c r="U12" t="s">
+        <v>65</v>
+      </c>
+      <c r="V12" t="s">
         <v>66</v>
       </c>
-      <c r="V12" t="s">
-        <v>67</v>
-      </c>
       <c r="W12" t="s">
+        <v>44</v>
+      </c>
+      <c r="X12" t="s">
         <v>46</v>
-      </c>
-      <c r="X12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13">
         <v>21193</v>
@@ -2805,54 +2808,54 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" t="s">
         <v>71</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>72</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" t="s">
         <v>73</v>
       </c>
-      <c r="L13" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>74</v>
-      </c>
-      <c r="O13" t="s">
-        <v>75</v>
       </c>
       <c r="P13" t="s">
         <v>12</v>
       </c>
       <c r="Q13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T13" t="s">
+        <v>44</v>
+      </c>
+      <c r="U13" t="s">
         <v>46</v>
-      </c>
-      <c r="U13" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14">
         <v>21193</v>
@@ -2870,60 +2873,60 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I14" t="s">
         <v>51</v>
       </c>
-      <c r="I14" t="s">
-        <v>52</v>
-      </c>
       <c r="J14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L14" t="s">
+        <v>56</v>
+      </c>
+      <c r="M14" t="s">
         <v>57</v>
       </c>
-      <c r="M14" t="s">
-        <v>58</v>
-      </c>
       <c r="N14" t="s">
+        <v>77</v>
+      </c>
+      <c r="O14" t="s">
         <v>78</v>
       </c>
-      <c r="O14" t="s">
-        <v>79</v>
-      </c>
       <c r="P14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q14" t="s">
         <v>12</v>
       </c>
       <c r="R14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T14" t="s">
+        <v>65</v>
+      </c>
+      <c r="U14" t="s">
         <v>66</v>
       </c>
-      <c r="U14" t="s">
-        <v>67</v>
-      </c>
       <c r="V14" t="s">
+        <v>44</v>
+      </c>
+      <c r="W14" t="s">
         <v>46</v>
-      </c>
-      <c r="W14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15">
         <v>21193</v>
@@ -2941,54 +2944,54 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" t="s">
         <v>51</v>
       </c>
-      <c r="J15" t="s">
-        <v>52</v>
-      </c>
       <c r="K15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N15" t="s">
         <v>57</v>
       </c>
-      <c r="N15" t="s">
-        <v>58</v>
-      </c>
       <c r="O15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q15" t="s">
         <v>12</v>
       </c>
       <c r="R15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T15" t="s">
+        <v>44</v>
+      </c>
+      <c r="U15" t="s">
         <v>46</v>
-      </c>
-      <c r="U15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:28">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16">
         <v>21193</v>
@@ -3006,75 +3009,75 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" t="s">
         <v>49</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" t="s">
         <v>50</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+      <c r="L16" t="s">
         <v>84</v>
       </c>
-      <c r="J16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
+        <v>53</v>
+      </c>
+      <c r="N16" t="s">
+        <v>54</v>
+      </c>
+      <c r="O16" t="s">
+        <v>102</v>
+      </c>
+      <c r="P16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R16" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16" t="s">
         <v>85</v>
       </c>
-      <c r="M16" t="s">
-        <v>54</v>
-      </c>
-      <c r="N16" t="s">
-        <v>55</v>
-      </c>
-      <c r="O16" t="s">
-        <v>103</v>
-      </c>
-      <c r="P16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="T16" t="s">
         <v>58</v>
       </c>
-      <c r="R16" t="s">
-        <v>33</v>
-      </c>
-      <c r="S16" t="s">
-        <v>86</v>
-      </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
+        <v>60</v>
+      </c>
+      <c r="V16" t="s">
         <v>59</v>
       </c>
-      <c r="U16" t="s">
-        <v>61</v>
-      </c>
-      <c r="V16" t="s">
-        <v>60</v>
-      </c>
       <c r="W16" t="s">
+        <v>88</v>
+      </c>
+      <c r="X16" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB16" t="s">
         <v>89</v>
-      </c>
-      <c r="X16" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y16" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA16" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17">
         <v>21193</v>
@@ -3092,45 +3095,45 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" t="s">
         <v>109</v>
       </c>
-      <c r="I17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" t="s">
-        <v>62</v>
-      </c>
-      <c r="L17" t="s">
-        <v>110</v>
-      </c>
       <c r="M17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" t="s">
         <v>66</v>
       </c>
-      <c r="P17" t="s">
-        <v>67</v>
-      </c>
       <c r="Q17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B18">
         <v>21193</v>
@@ -3148,42 +3151,42 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" t="s">
         <v>109</v>
       </c>
-      <c r="J18" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" t="s">
-        <v>62</v>
-      </c>
-      <c r="L18" t="s">
-        <v>110</v>
-      </c>
       <c r="M18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B19">
         <v>21193</v>
@@ -3201,48 +3204,48 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" t="s">
         <v>109</v>
       </c>
-      <c r="J19" t="s">
-        <v>39</v>
-      </c>
-      <c r="K19" t="s">
-        <v>62</v>
-      </c>
-      <c r="L19" t="s">
-        <v>110</v>
-      </c>
       <c r="M19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P19" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q19" t="s">
         <v>66</v>
       </c>
-      <c r="Q19" t="s">
-        <v>67</v>
-      </c>
       <c r="R19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20">
         <v>21193</v>
@@ -3260,39 +3263,39 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I20" t="s">
         <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="N20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21">
         <v>21193</v>
@@ -3310,48 +3313,48 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J21" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="L21" t="s">
+        <v>61</v>
+      </c>
+      <c r="M21" t="s">
         <v>109</v>
       </c>
-      <c r="J21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K21" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" t="s">
-        <v>62</v>
-      </c>
-      <c r="M21" t="s">
-        <v>110</v>
-      </c>
       <c r="N21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P21" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q21" t="s">
         <v>66</v>
       </c>
-      <c r="Q21" t="s">
-        <v>67</v>
-      </c>
       <c r="R21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:45">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22">
         <v>21193</v>
@@ -3485,13 +3488,10 @@
       <c r="AS22" t="s">
         <v>46</v>
       </c>
-      <c r="AT22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" customFormat="1" spans="1:30">
+    </row>
+    <row r="23" customFormat="1" spans="1:32">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23">
         <v>21193</v>
@@ -3509,81 +3509,87 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" t="s">
         <v>49</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>50</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>51</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>52</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>53</v>
       </c>
-      <c r="L23" t="s">
-        <v>54</v>
-      </c>
       <c r="M23" t="s">
+        <v>55</v>
+      </c>
+      <c r="N23" t="s">
         <v>56</v>
       </c>
-      <c r="N23" t="s">
+      <c r="O23" t="s">
         <v>57</v>
       </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q23" t="s">
         <v>58</v>
       </c>
-      <c r="P23" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>59</v>
       </c>
-      <c r="R23" t="s">
+      <c r="S23" t="s">
         <v>60</v>
       </c>
-      <c r="S23" t="s">
-        <v>61</v>
-      </c>
       <c r="T23" t="s">
+        <v>62</v>
+      </c>
+      <c r="U23" t="s">
         <v>63</v>
       </c>
-      <c r="U23" t="s">
+      <c r="V23" t="s">
         <v>64</v>
       </c>
-      <c r="V23" t="s">
+      <c r="W23" t="s">
         <v>65</v>
       </c>
-      <c r="W23" t="s">
+      <c r="X23" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y23" t="s">
         <v>66</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD23" t="s">
         <v>46</v>
       </c>
-      <c r="Y23" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC23" t="s">
+      <c r="AE23" t="s">
         <v>118</v>
       </c>
-      <c r="AD23" t="s">
-        <v>47</v>
+      <c r="AF23" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:31">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B24">
         <v>21193</v>
@@ -3601,84 +3607,84 @@
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" t="s">
         <v>51</v>
       </c>
-      <c r="I24" t="s">
-        <v>52</v>
-      </c>
       <c r="J24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" t="s">
+        <v>72</v>
+      </c>
+      <c r="L24" t="s">
         <v>56</v>
       </c>
-      <c r="K24" t="s">
-        <v>73</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>57</v>
       </c>
-      <c r="M24" t="s">
-        <v>58</v>
-      </c>
       <c r="N24" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24" t="s">
         <v>78</v>
       </c>
-      <c r="O24" t="s">
-        <v>79</v>
-      </c>
       <c r="P24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R24" t="s">
         <v>12</v>
       </c>
       <c r="S24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T24" t="s">
+        <v>62</v>
+      </c>
+      <c r="U24" t="s">
         <v>63</v>
       </c>
-      <c r="U24" t="s">
+      <c r="V24" t="s">
         <v>64</v>
       </c>
-      <c r="V24" t="s">
+      <c r="W24" t="s">
         <v>65</v>
       </c>
-      <c r="W24" t="s">
+      <c r="X24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y24" t="s">
         <v>66</v>
       </c>
-      <c r="X24" t="s">
+      <c r="Z24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>117</v>
+      </c>
+      <c r="AE24" t="s">
         <v>46</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>117</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:27">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B25">
         <v>21193</v>
@@ -3696,72 +3702,72 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J25" t="s">
         <v>71</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>72</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" t="s">
+        <v>57</v>
+      </c>
+      <c r="N25" t="s">
         <v>73</v>
       </c>
-      <c r="L25" t="s">
-        <v>57</v>
-      </c>
-      <c r="M25" t="s">
-        <v>58</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="O25" t="s">
+        <v>59</v>
+      </c>
+      <c r="P25" t="s">
         <v>74</v>
-      </c>
-      <c r="O25" t="s">
-        <v>60</v>
-      </c>
-      <c r="P25" t="s">
-        <v>75</v>
       </c>
       <c r="Q25" t="s">
         <v>12</v>
       </c>
       <c r="R25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T25" t="s">
+        <v>63</v>
+      </c>
+      <c r="U25" t="s">
         <v>64</v>
       </c>
-      <c r="U25" t="s">
-        <v>65</v>
-      </c>
       <c r="V25" t="s">
+        <v>44</v>
+      </c>
+      <c r="W25" t="s">
+        <v>67</v>
+      </c>
+      <c r="X25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA25" t="s">
         <v>46</v>
       </c>
-      <c r="W25" t="s">
-        <v>68</v>
-      </c>
-      <c r="X25" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" spans="1:36">
+    </row>
+    <row r="26" customFormat="1" spans="1:38">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B26">
         <v>21193</v>
@@ -3779,94 +3785,100 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" t="s">
         <v>49</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
+        <v>83</v>
+      </c>
+      <c r="J26" t="s">
         <v>50</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" t="s">
         <v>84</v>
       </c>
-      <c r="J26" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26" t="s">
-        <v>52</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
+        <v>53</v>
+      </c>
+      <c r="N26" t="s">
+        <v>55</v>
+      </c>
+      <c r="O26" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R26" t="s">
         <v>85</v>
       </c>
-      <c r="M26" t="s">
-        <v>54</v>
-      </c>
-      <c r="N26" t="s">
-        <v>56</v>
-      </c>
-      <c r="O26" t="s">
-        <v>57</v>
-      </c>
-      <c r="P26" t="s">
+      <c r="S26" t="s">
         <v>58</v>
       </c>
-      <c r="Q26" t="s">
-        <v>33</v>
-      </c>
-      <c r="R26" t="s">
+      <c r="T26" t="s">
+        <v>59</v>
+      </c>
+      <c r="U26" t="s">
+        <v>60</v>
+      </c>
+      <c r="V26" t="s">
         <v>86</v>
       </c>
-      <c r="S26" t="s">
-        <v>59</v>
-      </c>
-      <c r="T26" t="s">
-        <v>60</v>
-      </c>
-      <c r="U26" t="s">
-        <v>61</v>
-      </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>87</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y26" t="s">
         <v>88</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Z26" t="s">
         <v>63</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="AA26" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD26" t="s">
         <v>89</v>
       </c>
-      <c r="Z26" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB26" t="s">
+      <c r="AE26" t="s">
         <v>66</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="AF26" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI26" t="s">
+        <v>117</v>
+      </c>
+      <c r="AJ26" t="s">
         <v>46</v>
       </c>
-      <c r="AD26" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG26" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH26" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI26" t="s">
+      <c r="AK26" t="s">
         <v>118</v>
       </c>
-      <c r="AJ26" t="s">
-        <v>47</v>
+      <c r="AL26" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3880,8 +3892,8 @@
   <sheetPr/>
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3895,419 +3907,419 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B2">
         <v>3795</v>
       </c>
       <c r="C2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <v>3743</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B4">
         <v>14105</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="N4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="O4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5">
         <v>14103</v>
       </c>
       <c r="C5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G5" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>147813</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7">
         <v>147809</v>
       </c>
       <c r="C7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H7" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8">
         <v>147807</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B9">
         <v>147805</v>
       </c>
       <c r="C9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B10">
         <v>147801</v>
       </c>
       <c r="C10" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J10" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B11">
         <v>147799</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J11" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K11" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B12">
         <v>147797</v>
       </c>
       <c r="C12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B13">
         <v>147795</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H13" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14">
         <v>147793</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G14" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B15">
         <v>147789</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F15" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="G15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H15" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="I15" t="s">
         <v>148</v>
@@ -4315,550 +4327,595 @@
       <c r="J15" t="s">
         <v>149</v>
       </c>
+      <c r="K15" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B16">
         <v>147787</v>
       </c>
       <c r="C16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B17">
         <v>147785</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H17" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B18">
         <v>147783</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D18" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F18" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H18" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I18" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B19">
         <v>147781</v>
       </c>
       <c r="C19" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H19" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B20">
         <v>147779</v>
       </c>
       <c r="C20" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F20" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G20" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H20" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I20" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B21">
         <v>147771</v>
       </c>
       <c r="C21" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D21" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F21" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H21" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J21" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K21" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B22">
         <v>147763</v>
       </c>
       <c r="C22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F22" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H22" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L22" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B23">
         <v>147761</v>
       </c>
       <c r="C23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="I23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J23" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B24">
         <v>147759</v>
       </c>
       <c r="C24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G24" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H24" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I24" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K24" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B25">
         <v>147757</v>
       </c>
       <c r="C25" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G25" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J25" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26">
         <v>148425</v>
       </c>
       <c r="C26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D26" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E26" t="s">
         <v>147</v>
       </c>
       <c r="F26" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G26" t="s">
+        <v>157</v>
+      </c>
+      <c r="H26" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B27">
         <v>148343</v>
       </c>
       <c r="C27" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D27" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E27" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="F27" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="G27" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="H27" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="J27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B28">
         <v>148341</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D28" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E28" t="s">
         <v>147</v>
       </c>
       <c r="F28" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G28" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B29">
         <v>148339</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D29" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E29" t="s">
         <v>147</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G29" t="s">
+        <v>157</v>
+      </c>
+      <c r="H29" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="I29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B30">
         <v>148337</v>
       </c>
       <c r="C30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" t="s">
         <v>147</v>
-      </c>
-      <c r="E30" t="s">
-        <v>148</v>
       </c>
       <c r="F30" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B31">
         <v>148335</v>
       </c>
       <c r="C31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
         <v>147</v>
-      </c>
-      <c r="E31" t="s">
-        <v>148</v>
       </c>
       <c r="F31" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="G31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B32">
         <v>148333</v>
       </c>
       <c r="C32" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
         <v>147</v>
       </c>
       <c r="F32" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G32" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B33">
         <v>148327</v>
       </c>
       <c r="C33" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E33" t="s">
         <v>147</v>
       </c>
       <c r="F33" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G33" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B34">
         <v>148325</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E34" t="s">
         <v>147</v>
       </c>
       <c r="F34" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="G34" t="s">
+        <v>157</v>
+      </c>
+      <c r="H34" t="s">
         <v>149</v>
       </c>
-      <c r="H34" t="s">
-        <v>174</v>
+      <c r="I34" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -4872,8 +4929,8 @@
   <sheetPr/>
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -4883,12 +4940,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B2">
         <v>581</v>
@@ -4897,357 +4954,360 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K2" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="L2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B3">
         <v>1571285</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
         <v>51</v>
       </c>
-      <c r="F3" t="s">
-        <v>52</v>
-      </c>
       <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>57</v>
       </c>
-      <c r="J3" t="s">
-        <v>58</v>
-      </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M3" t="s">
         <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B4">
         <v>1571283</v>
       </c>
       <c r="C4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
         <v>51</v>
       </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
         <v>56</v>
       </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>57</v>
       </c>
-      <c r="I4" t="s">
-        <v>58</v>
-      </c>
       <c r="J4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" t="s">
         <v>78</v>
       </c>
-      <c r="K4" t="s">
-        <v>79</v>
-      </c>
       <c r="L4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M4" t="s">
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>1566625</v>
       </c>
       <c r="C5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
         <v>71</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>72</v>
       </c>
-      <c r="G5" t="s">
-        <v>73</v>
-      </c>
       <c r="H5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s">
         <v>57</v>
       </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
       <c r="J5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="K5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="O5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B6">
         <v>1566605</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
         <v>51</v>
       </c>
-      <c r="E6" t="s">
-        <v>52</v>
-      </c>
       <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>57</v>
       </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
       <c r="I6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="M6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B7">
         <v>1571285</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E7" t="s">
+        <v>208</v>
+      </c>
+      <c r="F7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" t="s">
         <v>206</v>
-      </c>
-      <c r="F7" t="s">
-        <v>207</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B8">
         <v>1571283</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F8" t="s">
+        <v>209</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" t="s">
         <v>206</v>
-      </c>
-      <c r="F8" t="s">
-        <v>207</v>
-      </c>
-      <c r="G8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H8" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B9">
         <v>1566605</v>
       </c>
       <c r="C9" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E9" t="s">
+        <v>208</v>
+      </c>
+      <c r="F9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
         <v>206</v>
-      </c>
-      <c r="F9" t="s">
-        <v>207</v>
-      </c>
-      <c r="G9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B10">
         <v>23349</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G10" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B11">
         <v>23520</v>
       </c>
       <c r="C11" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E11" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B12">
         <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D12" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E12" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
face liveliness script and grid action fix and proctoring path change
</commit_message>
<xml_diff>
--- a/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
+++ b/PythonWorkingScripts_InputData/UI/Assessment/Grid_Actions_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16575" windowHeight="7500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="10580"/>
   </bookViews>
   <sheets>
     <sheet name="assessment_grid_actions" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="227">
   <si>
     <t>TestCases</t>
   </si>
@@ -173,6 +173,9 @@
     <t>Dry run evaluation through AI</t>
   </si>
   <si>
+    <t>Enable Reminder</t>
+  </si>
+  <si>
     <t>Assessment applicants (Attended not evaluated)</t>
   </si>
   <si>
@@ -387,6 +390,9 @@
   </si>
   <si>
     <t>Launch Evaluation Container</t>
+  </si>
+  <si>
+    <t>Launch Evaluation Test User Containers</t>
   </si>
   <si>
     <t>View And Download Candidate DevOPS Answer</t>
@@ -1666,15 +1672,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AT26"/>
+  <dimension ref="A1:AU26"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="103" topLeftCell="X8" workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+    <sheetView tabSelected="1" zoomScale="103" zoomScaleNormal="103" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="28.8857142857143" customWidth="1"/>
+    <col min="1" max="1" width="28.8828125" customWidth="1"/>
     <col min="2" max="3" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1698,7 +1704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:46">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1834,10 +1840,13 @@
       <c r="AS2" t="s">
         <v>46</v>
       </c>
+      <c r="AT2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="3" customFormat="1" spans="1:31">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3">
         <v>21193</v>
@@ -1855,76 +1864,76 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q3" t="s">
         <v>31</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="T3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="U3" t="s">
         <v>37</v>
       </c>
       <c r="V3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Y3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA3" t="s">
         <v>44</v>
       </c>
       <c r="AB3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AC3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AD3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AE3" t="s">
         <v>46</v>
@@ -1932,7 +1941,7 @@
     </row>
     <row r="4" customFormat="1" spans="1:25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B4">
         <v>21193</v>
@@ -1950,58 +1959,58 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q4" t="s">
         <v>12</v>
       </c>
       <c r="R4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S4" t="s">
         <v>28</v>
       </c>
       <c r="T4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V4" t="s">
         <v>44</v>
       </c>
       <c r="W4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Y4" t="s">
         <v>46</v>
@@ -2009,7 +2018,7 @@
     </row>
     <row r="5" customFormat="1" spans="1:30">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B5">
         <v>21193</v>
@@ -2027,37 +2036,37 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R5" t="s">
         <v>12</v>
@@ -2066,34 +2075,34 @@
         <v>37</v>
       </c>
       <c r="T5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="V5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="W5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="X5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Y5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Z5" t="s">
         <v>44</v>
       </c>
       <c r="AA5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AB5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AD5" t="s">
         <v>46</v>
@@ -2101,7 +2110,7 @@
     </row>
     <row r="6" customFormat="1" spans="1:28">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B6">
         <v>21193</v>
@@ -2119,37 +2128,37 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R6" t="s">
         <v>12</v>
@@ -2158,28 +2167,28 @@
         <v>37</v>
       </c>
       <c r="T6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="U6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="V6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="W6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="X6" t="s">
         <v>44</v>
       </c>
       <c r="Y6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB6" t="s">
         <v>46</v>
@@ -2187,7 +2196,7 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B7">
         <v>21193</v>
@@ -2205,102 +2214,102 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
         <v>31</v>
       </c>
       <c r="S7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="W7" t="s">
         <v>37</v>
       </c>
       <c r="X7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Y7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="Z7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AA7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AB7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AC7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AD7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AE7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AF7" t="s">
         <v>44</v>
       </c>
       <c r="AG7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AH7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AJ7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AK7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:46">
+    <row r="8" customFormat="1" spans="1:47">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>21381</v>
@@ -2399,7 +2408,7 @@
         <v>34</v>
       </c>
       <c r="AH8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AI8" t="s">
         <v>35</v>
@@ -2437,10 +2446,13 @@
       <c r="AT8" t="s">
         <v>46</v>
       </c>
+      <c r="AU8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" customFormat="1" spans="1:26">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B9">
         <v>21381</v>
@@ -2458,61 +2470,61 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q9" t="s">
         <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S9" t="s">
         <v>28</v>
       </c>
       <c r="T9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="V9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W9" t="s">
         <v>44</v>
       </c>
       <c r="X9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Y9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Z9" t="s">
         <v>46</v>
@@ -2520,7 +2532,7 @@
     </row>
     <row r="10" customFormat="1" spans="1:32">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B10">
         <v>21381</v>
@@ -2538,87 +2550,87 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P10" t="s">
         <v>31</v>
       </c>
       <c r="Q10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="U10" t="s">
         <v>37</v>
       </c>
       <c r="V10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="W10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="X10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Y10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Z10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AB10" t="s">
         <v>44</v>
       </c>
       <c r="AC10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AD10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AE10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AF10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B11">
         <v>21193</v>
@@ -2687,7 +2699,7 @@
         <v>26</v>
       </c>
       <c r="X11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Y11" t="s">
         <v>29</v>
@@ -2696,13 +2708,13 @@
         <v>31</v>
       </c>
       <c r="AA11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AB11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AC11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AD11" t="s">
         <v>28</v>
@@ -2713,10 +2725,13 @@
       <c r="AF11" t="s">
         <v>45</v>
       </c>
+      <c r="AG11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B12">
         <v>21193</v>
@@ -2734,52 +2749,52 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q12" t="s">
         <v>31</v>
       </c>
       <c r="R12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S12" t="s">
+        <v>61</v>
+      </c>
+      <c r="T12" t="s">
         <v>60</v>
       </c>
-      <c r="T12" t="s">
-        <v>59</v>
-      </c>
       <c r="U12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W12" t="s">
         <v>44</v>
@@ -2790,7 +2805,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B13">
         <v>21193</v>
@@ -2808,40 +2823,40 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K13" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L13" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
         <v>12</v>
       </c>
       <c r="Q13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="R13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S13" t="s">
         <v>28</v>
@@ -2855,7 +2870,7 @@
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B14">
         <v>21193</v>
@@ -2873,49 +2888,49 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q14" t="s">
         <v>12</v>
       </c>
       <c r="R14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="T14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V14" t="s">
         <v>44</v>
@@ -2926,7 +2941,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B15">
         <v>21193</v>
@@ -2944,43 +2959,43 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="L15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="M15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="P15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q15" t="s">
         <v>12</v>
       </c>
       <c r="R15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T15" t="s">
         <v>44</v>
@@ -2991,7 +3006,7 @@
     </row>
     <row r="16" spans="1:28">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B16">
         <v>21193</v>
@@ -3009,61 +3024,61 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="R16" t="s">
         <v>31</v>
       </c>
       <c r="S16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U16" t="s">
+        <v>61</v>
+      </c>
+      <c r="V16" t="s">
         <v>60</v>
       </c>
-      <c r="V16" t="s">
-        <v>59</v>
-      </c>
       <c r="W16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="X16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z16" t="s">
         <v>44</v>
@@ -3072,12 +3087,12 @@
         <v>46</v>
       </c>
       <c r="AB16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B17">
         <v>21193</v>
@@ -3095,34 +3110,34 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H17" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J17" t="s">
         <v>37</v>
       </c>
       <c r="K17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q17" t="s">
         <v>46</v>
@@ -3133,7 +3148,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B18">
         <v>21193</v>
@@ -3151,31 +3166,31 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J18" t="s">
         <v>37</v>
       </c>
       <c r="K18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P18" t="s">
         <v>46</v>
@@ -3186,7 +3201,7 @@
     </row>
     <row r="19" spans="1:19">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19">
         <v>21193</v>
@@ -3204,37 +3219,37 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H19" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J19" t="s">
         <v>37</v>
       </c>
       <c r="K19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R19" t="s">
         <v>46</v>
@@ -3245,7 +3260,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B20">
         <v>21193</v>
@@ -3263,28 +3278,28 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
         <v>12</v>
       </c>
       <c r="J20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="L20" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M20" t="s">
         <v>28</v>
       </c>
       <c r="N20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O20" t="s">
         <v>46</v>
@@ -3295,7 +3310,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B21">
         <v>21193</v>
@@ -3313,37 +3328,37 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K21" t="s">
         <v>37</v>
       </c>
       <c r="L21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="N21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O21" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="P21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R21" t="s">
         <v>46</v>
@@ -3352,9 +3367,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:45">
+    <row r="22" spans="1:46">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B22">
         <v>21193</v>
@@ -3488,10 +3503,13 @@
       <c r="AS22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" customFormat="1" spans="1:32">
+      <c r="AT22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" spans="1:33">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23">
         <v>21193</v>
@@ -3509,87 +3527,90 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="M23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P23" t="s">
         <v>31</v>
       </c>
       <c r="Q23" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="S23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="T23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X23" t="s">
         <v>44</v>
       </c>
       <c r="Y23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AC23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AD23" t="s">
         <v>46</v>
       </c>
       <c r="AE23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AF23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" customFormat="1" spans="1:31">
+        <v>120</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" spans="1:32">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B24">
         <v>21193</v>
@@ -3607,84 +3628,87 @@
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M24" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="P24" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q24" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="R24" t="s">
         <v>12</v>
       </c>
       <c r="S24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="T24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U24" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="V24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="W24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X24" t="s">
         <v>44</v>
       </c>
       <c r="Y24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AB24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AC24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AD24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AE24" t="s">
         <v>46</v>
       </c>
+      <c r="AF24" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="25" customFormat="1" spans="1:27">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B25">
         <v>21193</v>
@@ -3702,72 +3726,72 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="M25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="N25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Q25" t="s">
         <v>12</v>
       </c>
       <c r="R25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="S25" t="s">
         <v>28</v>
       </c>
       <c r="T25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V25" t="s">
         <v>44</v>
       </c>
       <c r="W25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Y25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="Z25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AA25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" customFormat="1" spans="1:38">
+    <row r="26" customFormat="1" spans="1:39">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B26">
         <v>21193</v>
@@ -3785,100 +3809,103 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="P26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Q26" t="s">
         <v>31</v>
       </c>
       <c r="R26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="T26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="V26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="W26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="X26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Y26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="Z26" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AB26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AC26" t="s">
         <v>44</v>
       </c>
       <c r="AD26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AE26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AF26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AG26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AH26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AI26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="AJ26" t="s">
         <v>46</v>
       </c>
       <c r="AK26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="AL26" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3892,14 +3919,14 @@
   <sheetPr/>
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <cols>
-    <col min="1" max="1" width="18.2857142857143" customWidth="1"/>
-    <col min="2" max="2" width="16.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="18.2890625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -3907,1015 +3934,1015 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B2">
         <v>3795</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B3">
         <v>3743</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B4">
         <v>14105</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L4" t="s">
         <v>38</v>
       </c>
       <c r="M4" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="O4" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B5">
         <v>14103</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="I5" t="s">
         <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K5" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B6">
         <v>147813</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7">
         <v>147809</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>147807</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G8" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B9">
         <v>147805</v>
       </c>
       <c r="C9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B10">
         <v>147801</v>
       </c>
       <c r="C10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F10" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G10" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I10" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B11">
         <v>147799</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="I11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="J11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="K11" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <v>147797</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F12" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H12" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J12" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K12" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B13">
         <v>147795</v>
       </c>
       <c r="C13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14">
         <v>147793</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I14" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B15">
         <v>147789</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F15" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G15" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H15" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I15" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B16">
         <v>147787</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F16" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G16" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H16" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K16" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B17">
         <v>147785</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D17" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F17" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G17" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I17" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J17" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18">
         <v>147783</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G18" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I18" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B19">
         <v>147781</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B20">
         <v>147779</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D20" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E20" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F20" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G20" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H20" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J20" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B21">
         <v>147771</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F21" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H21" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K21" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B22">
         <v>147763</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D22" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E22" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G22" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H22" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J22" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K22" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B23">
         <v>147761</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D23" t="s">
+        <v>179</v>
+      </c>
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" t="s">
+        <v>155</v>
+      </c>
+      <c r="H23" t="s">
+        <v>159</v>
+      </c>
+      <c r="I23" t="s">
+        <v>151</v>
+      </c>
+      <c r="J23" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" t="s">
         <v>177</v>
-      </c>
-      <c r="E23" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" t="s">
-        <v>156</v>
-      </c>
-      <c r="G23" t="s">
-        <v>153</v>
-      </c>
-      <c r="H23" t="s">
-        <v>157</v>
-      </c>
-      <c r="I23" t="s">
-        <v>149</v>
-      </c>
-      <c r="J23" t="s">
-        <v>150</v>
-      </c>
-      <c r="K23" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B24">
         <v>147759</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H24" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J24" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K24" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B25">
         <v>147757</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F25" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H25" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J25" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K25" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B26">
         <v>148425</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E26" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F26" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G26" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H26" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I26" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B27">
         <v>148343</v>
       </c>
       <c r="C27" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E27" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F27" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H27" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="I27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B28">
         <v>148341</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E28" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G28" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H28" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B29">
         <v>148339</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E29" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F29" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G29" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H29" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I29" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B30">
         <v>148337</v>
       </c>
       <c r="C30" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F30" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G30" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B31">
         <v>148335</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E31" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G31" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B32">
         <v>148333</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F32" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G32" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B33">
         <v>148327</v>
       </c>
       <c r="C33" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F33" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G33" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H33" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I33" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B34">
         <v>148325</v>
       </c>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D34" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F34" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G34" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H34" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I34" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="J34" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4933,19 +4960,19 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>581</v>
@@ -4954,10 +4981,10 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -4969,345 +4996,345 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="K2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B3">
         <v>1571285</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M3" t="s">
         <v>12</v>
       </c>
       <c r="N3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="O3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B4">
         <v>1571283</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M4" t="s">
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B5">
         <v>1566625</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="K5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="O5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B6">
         <v>1566605</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I6" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
       </c>
       <c r="L6" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="M6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N6" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B7">
         <v>1571285</v>
       </c>
       <c r="C7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E7" t="s">
+        <v>210</v>
+      </c>
+      <c r="F7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
         <v>208</v>
-      </c>
-      <c r="F7" t="s">
-        <v>209</v>
-      </c>
-      <c r="G7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H7" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B8">
         <v>1571283</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E8" t="s">
+        <v>210</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" t="s">
         <v>208</v>
-      </c>
-      <c r="F8" t="s">
-        <v>209</v>
-      </c>
-      <c r="G8" t="s">
-        <v>86</v>
-      </c>
-      <c r="H8" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B9">
         <v>1566605</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D9" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" t="s">
         <v>208</v>
-      </c>
-      <c r="F9" t="s">
-        <v>209</v>
-      </c>
-      <c r="G9" t="s">
-        <v>86</v>
-      </c>
-      <c r="H9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B10">
         <v>23349</v>
       </c>
       <c r="C10" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E10" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F10" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G10" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B11">
         <v>23520</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E11" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G11" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B12">
         <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D12" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E12" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -5325,7 +5352,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.8"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>